<commit_message>
working on report, backup
</commit_message>
<xml_diff>
--- a/bin-pack-good.xlsx
+++ b/bin-pack-good.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="22755" windowHeight="10275" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="22755" windowHeight="10275"/>
   </bookViews>
   <sheets>
     <sheet name="bin-pack_12-06_21-51-52" sheetId="1" r:id="rId1"/>
     <sheet name="special" sheetId="2" r:id="rId2"/>
     <sheet name="PTAS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="28">
   <si>
     <t>Algorithm</t>
   </si>
@@ -63,21 +63,6 @@
     <t>Running a worst case for First Fit</t>
   </si>
   <si>
-    <t>BF-D</t>
-  </si>
-  <si>
-    <t>NF</t>
-  </si>
-  <si>
-    <t>NF-D</t>
-  </si>
-  <si>
-    <t>WF</t>
-  </si>
-  <si>
-    <t>WF-D</t>
-  </si>
-  <si>
     <t>Algo</t>
   </si>
   <si>
@@ -94,6 +79,27 @@
   </si>
   <si>
     <t>ptas_ff</t>
+  </si>
+  <si>
+    <t>Eps</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Next Fit</t>
+  </si>
+  <si>
+    <t>Next Fit Desc.</t>
+  </si>
+  <si>
+    <t>Worst Fit</t>
+  </si>
+  <si>
+    <t>Worst Fit Desc.</t>
+  </si>
+  <si>
+    <t>Best Fit Desc.</t>
   </si>
 </sst>
 </file>
@@ -635,6 +641,520 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Runtime of Bin-Packing Algorithms</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8797339098912335E-2"/>
+          <c:y val="0.13342070171172279"/>
+          <c:w val="0.88000805910699575"/>
+          <c:h val="0.78714481421070226"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'bin-pack_12-06_21-51-52'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Runtime (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'bin-pack_12-06_21-51-52'!$L$2:$L$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Next Fit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Next Fit Desc.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Worst Fit</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Worst Fit Desc.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Best Fit Desc.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'bin-pack_12-06_21-51-52'!$M$2:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.26924681249999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35089605468749985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.064718273437502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9753418582677149</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5234293046874985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="175708032"/>
+        <c:axId val="181548928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="175708032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="181548928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="181548928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100"/>
+                  <a:t>Average Clock Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.5048165756654112E-2"/>
+              <c:y val="0.34759565102216761"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="175708032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Approximation Ratio of Bin-Packing Algorithms</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'bin-pack_12-06_21-51-52'!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SOL/OPT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.0176542095495416E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'bin-pack_12-06_21-51-52'!$L$2:$L$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Next Fit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Next Fit Desc.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Worst Fit</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Worst Fit Desc.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Best Fit Desc.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'bin-pack_12-06_21-51-52'!$N$2:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.3333719531249995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2896800937500001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1715476796874995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0016893671875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0016411718749996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="150799872"/>
+        <c:axId val="150801408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="150799872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150801408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="150801408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Approximation Ratio (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1100"/>
+                  <a:t>SOL/OPT</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4317671360401437E-2"/>
+              <c:y val="0.29009816337862288"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150799872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -924,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N641"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +1453,7 @@
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -959,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -991,7 +1512,7 @@
         <v>1.0028950000000001</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="M2">
         <f>AVERAGE(D130:D257)</f>
@@ -1025,7 +1546,7 @@
         <v>1.001398</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="M3">
         <f>AVERAGE(D258:D385)</f>
@@ -1059,7 +1580,7 @@
         <v>1.00156</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M4">
         <f>AVERAGE(D386:D513)</f>
@@ -1093,7 +1614,7 @@
         <v>1.0011410000000001</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="M5">
         <f>AVERAGE(D514:D641)</f>
@@ -1127,7 +1648,7 @@
         <v>1.00118</v>
       </c>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="M6">
         <f>AVERAGE(D2:D129)</f>
@@ -14774,7 +15295,7 @@
         <v>1.002875</v>
       </c>
       <c r="H599" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="600" spans="1:8" x14ac:dyDescent="0.25">
@@ -15749,6 +16270,7 @@
     <sortCondition ref="B2:B641"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16101,15 +16623,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16132,12 +16654,21 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -16160,10 +16691,21 @@
       <c r="H2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0.1</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(D2:D33)</f>
+        <v>6.7290304687500004</v>
+      </c>
+      <c r="M2">
+        <f>AVERAGE(G2:G33)</f>
+        <v>1.0523554687500001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -16186,10 +16728,21 @@
       <c r="H3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0.01</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE(D34:D65)</f>
+        <v>6.9147025937500004</v>
+      </c>
+      <c r="M3">
+        <f>AVERAGE(G34:G65)</f>
+        <v>1.0069068750000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -16212,10 +16765,21 @@
       <c r="H4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1E-3</v>
+      </c>
+      <c r="L4">
+        <f>AVERAGE(D66:D97)</f>
+        <v>6.9374615312499985</v>
+      </c>
+      <c r="M4">
+        <f>AVERAGE(G66:G97)</f>
+        <v>1.0023653437499997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -16238,10 +16802,21 @@
       <c r="H5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>1E-4</v>
+      </c>
+      <c r="L5">
+        <f>AVERAGE(D98:D129)</f>
+        <v>6.9413392500000004</v>
+      </c>
+      <c r="M5">
+        <f>AVERAGE(G98:G129)</f>
+        <v>1.0015928125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -16265,9 +16840,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -16291,9 +16866,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -16317,9 +16892,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -16343,9 +16918,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -16369,9 +16944,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -16395,9 +16970,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -16421,9 +16996,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -16447,9 +17022,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -16473,9 +17048,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -16499,9 +17074,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -16527,7 +17102,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -16553,7 +17128,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -16579,7 +17154,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -16605,7 +17180,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -16631,7 +17206,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -16657,7 +17232,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -16683,7 +17258,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -16709,7 +17284,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -16735,7 +17310,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -16761,7 +17336,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -16787,7 +17362,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -16813,7 +17388,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -16839,7 +17414,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -16865,7 +17440,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -16891,7 +17466,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -16917,7 +17492,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -16943,7 +17518,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -16969,7 +17544,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -16995,7 +17570,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -17021,7 +17596,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -17047,7 +17622,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -17073,7 +17648,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -17099,7 +17674,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -17125,7 +17700,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
@@ -17151,7 +17726,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -17177,7 +17752,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
@@ -17203,7 +17778,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -17229,7 +17804,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -17255,7 +17830,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -17281,7 +17856,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
@@ -17307,7 +17882,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
@@ -17333,7 +17908,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
@@ -17359,7 +17934,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
@@ -17385,7 +17960,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -17411,7 +17986,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -17437,7 +18012,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
@@ -17463,7 +18038,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
@@ -17489,7 +18064,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
@@ -17515,7 +18090,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
@@ -17541,7 +18116,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
@@ -17567,7 +18142,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -17593,7 +18168,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
@@ -17619,7 +18194,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
@@ -17645,7 +18220,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -17671,7 +18246,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
@@ -17697,7 +18272,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
@@ -17723,7 +18298,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
@@ -17749,7 +18324,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
@@ -17775,7 +18350,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
@@ -17801,7 +18376,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
@@ -17827,7 +18402,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -17853,7 +18428,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
@@ -17879,7 +18454,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -17905,7 +18480,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
@@ -17931,7 +18506,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
@@ -17957,7 +18532,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B72" t="s">
         <v>10</v>
@@ -17983,7 +18558,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
@@ -18009,7 +18584,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
@@ -18035,7 +18610,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
@@ -18061,7 +18636,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
@@ -18087,7 +18662,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
@@ -18113,7 +18688,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
         <v>10</v>
@@ -18139,7 +18714,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B79" t="s">
         <v>10</v>
@@ -18165,7 +18740,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B80" t="s">
         <v>10</v>
@@ -18191,7 +18766,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
@@ -18217,7 +18792,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B82" t="s">
         <v>10</v>
@@ -18243,7 +18818,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B83" t="s">
         <v>10</v>
@@ -18269,7 +18844,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B84" t="s">
         <v>10</v>
@@ -18295,7 +18870,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B85" t="s">
         <v>10</v>
@@ -18321,7 +18896,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B86" t="s">
         <v>10</v>
@@ -18347,7 +18922,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B87" t="s">
         <v>10</v>
@@ -18373,7 +18948,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B88" t="s">
         <v>10</v>
@@ -18399,7 +18974,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B89" t="s">
         <v>10</v>
@@ -18425,7 +19000,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B90" t="s">
         <v>10</v>
@@ -18451,7 +19026,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
@@ -18477,7 +19052,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B92" t="s">
         <v>10</v>
@@ -18503,7 +19078,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B93" t="s">
         <v>10</v>
@@ -18529,7 +19104,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
@@ -18555,7 +19130,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B95" t="s">
         <v>10</v>
@@ -18581,7 +19156,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B96" t="s">
         <v>10</v>
@@ -18607,7 +19182,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B97" t="s">
         <v>10</v>
@@ -18633,7 +19208,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B98" t="s">
         <v>10</v>
@@ -18659,7 +19234,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B99" t="s">
         <v>10</v>
@@ -18685,7 +19260,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B100" t="s">
         <v>10</v>
@@ -18711,7 +19286,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B101" t="s">
         <v>10</v>
@@ -18737,7 +19312,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B102" t="s">
         <v>10</v>
@@ -18763,7 +19338,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B103" t="s">
         <v>10</v>
@@ -18789,7 +19364,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B104" t="s">
         <v>10</v>
@@ -18815,7 +19390,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B105" t="s">
         <v>10</v>
@@ -18841,7 +19416,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B106" t="s">
         <v>10</v>
@@ -18867,7 +19442,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B107" t="s">
         <v>10</v>
@@ -18893,7 +19468,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B108" t="s">
         <v>10</v>
@@ -18919,7 +19494,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B109" t="s">
         <v>10</v>
@@ -18945,7 +19520,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B110" t="s">
         <v>10</v>
@@ -18971,7 +19546,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -18997,7 +19572,7 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B112" t="s">
         <v>10</v>
@@ -19023,7 +19598,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B113" t="s">
         <v>10</v>
@@ -19049,7 +19624,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B114" t="s">
         <v>10</v>
@@ -19075,7 +19650,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B115" t="s">
         <v>10</v>
@@ -19101,7 +19676,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B116" t="s">
         <v>10</v>
@@ -19127,7 +19702,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B117" t="s">
         <v>10</v>
@@ -19153,7 +19728,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B118" t="s">
         <v>10</v>
@@ -19179,7 +19754,7 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B119" t="s">
         <v>10</v>
@@ -19205,7 +19780,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B120" t="s">
         <v>10</v>
@@ -19231,7 +19806,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B121" t="s">
         <v>10</v>
@@ -19257,7 +19832,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B122" t="s">
         <v>10</v>
@@ -19283,7 +19858,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B123" t="s">
         <v>10</v>
@@ -19309,7 +19884,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B124" t="s">
         <v>10</v>
@@ -19335,7 +19910,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B125" t="s">
         <v>10</v>
@@ -19361,7 +19936,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
         <v>10</v>
@@ -19387,7 +19962,7 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B127" t="s">
         <v>10</v>
@@ -19413,7 +19988,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B128" t="s">
         <v>10</v>
@@ -19439,7 +20014,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B129" t="s">
         <v>10</v>

</xml_diff>